<commit_message>
Added data and examples to the AllFunctions Template
</commit_message>
<xml_diff>
--- a/templates/AllFunctions/0.RawData/ParticipantData.xlsx
+++ b/templates/AllFunctions/0.RawData/ParticipantData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1003161\Documents\EXPERIENCELAB\ExperienceLabPipeline\templates\AllFunctions\0.RawData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\EXP_Lab\ExperienceLabPipelineGit\templates\AllFunctions\0.RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7819D2EB-158A-4801-A954-5BAB37332863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A053AF-38C5-4648-9598-C6A27AEDD7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="3825" windowWidth="38700" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51105" yWindow="2340" windowWidth="23460" windowHeight="17490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Participant</t>
   </si>
@@ -61,6 +61,24 @@
   </si>
   <si>
     <t>In</t>
+  </si>
+  <si>
+    <t>EDA</t>
+  </si>
+  <si>
+    <t>Indoor</t>
+  </si>
+  <si>
+    <t>Strava</t>
+  </si>
+  <si>
+    <t>16-Aug-2019 10:33:00</t>
+  </si>
+  <si>
+    <t>16-Aug-2019 10:50:05</t>
+  </si>
+  <si>
+    <t>DataType</t>
   </si>
 </sst>
 </file>
@@ -393,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E8" sqref="E7:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,7 +425,7 @@
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,8 +444,11 @@
       <c r="F1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -447,58 +468,99 @@
       <c r="F2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D4" si="0">(HOUR($C3-$B3)*3600)+(MINUTE($C3-$B3)*60)+(SECOND($C3-$B3))</f>
+        <v>2280</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="0"/>
+        <v>1025</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="2"/>

</xml_diff>